<commit_message>
Handle mistakenly resolved checks
</commit_message>
<xml_diff>
--- a/OPID/Uploads/Voided Checks August 2017.xlsx
+++ b/OPID/Uploads/Voided Checks August 2017.xlsx
@@ -770,7 +770,7 @@
   <dimension ref="A1:G128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="C128" sqref="C128"/>
+      <selection activeCell="B130" sqref="B130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2155,12 +2155,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="10">
-        <v>42955</v>
-      </c>
-      <c r="C128">
-        <v>79873</v>
-      </c>
+      <c r="A128" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>